<commit_message>
Arreglando matrices + AS enteros
</commit_message>
<xml_diff>
--- a/Compiladores-G19/matrices.xlsx
+++ b/Compiladores-G19/matrices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Facultad\Compiladores-G19\Compiladores-G19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D3C5A4-EA87-4C67-BF87-A581A1339EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C5CA7D-578B-431A-AFA5-4A33AC833903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="-75" windowWidth="21600" windowHeight="11295" xr2:uid="{B262041E-6529-4A45-91DA-BFC8946D9AB8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B262041E-6529-4A45-91DA-BFC8946D9AB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -552,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C414953C-C430-47AB-9AE2-E37D39AE491A}">
   <dimension ref="A1:XFD44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>